<commit_message>
TOD-E norms run, POM rescale, 24 cell demo strat
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lske_sum-raw-ss-lookup-tabbed.xlsx
@@ -12,7 +12,10 @@
     <sheet name="5.8-5.11" sheetId="3" r:id="rId3"/>
     <sheet name="6.0-6.5" sheetId="4" r:id="rId4"/>
     <sheet name="6.6-6.11" sheetId="5" r:id="rId5"/>
-    <sheet name="7.0-9.3" sheetId="6" r:id="rId6"/>
+    <sheet name="7.0-7.5" sheetId="6" r:id="rId6"/>
+    <sheet name="7.6-7.11" sheetId="7" r:id="rId7"/>
+    <sheet name="8.0-8.5" sheetId="8" r:id="rId8"/>
+    <sheet name="8.6-9.3" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1824,7 +1827,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -1832,7 +1835,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -1840,7 +1843,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
@@ -1848,7 +1851,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
@@ -1856,7 +1859,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -1864,7 +1867,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8">
@@ -1872,7 +1875,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
@@ -1880,7 +1883,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10">
@@ -1888,7 +1891,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
@@ -1896,7 +1899,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12">
@@ -1904,7 +1907,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13">
@@ -1912,7 +1915,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
@@ -1920,7 +1923,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -1928,7 +1931,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -1936,7 +1939,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -1944,7 +1947,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -1952,7 +1955,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19">
@@ -1960,7 +1963,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20">
@@ -1968,7 +1971,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21">
@@ -1976,7 +1979,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22">
@@ -1984,7 +1987,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23">
@@ -1992,7 +1995,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24">
@@ -2000,7 +2003,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25">
@@ -2008,7 +2011,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26">
@@ -2016,7 +2019,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27">
@@ -2024,7 +2027,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28">
@@ -2032,7 +2035,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29">
@@ -2040,7 +2043,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30">
@@ -2048,7 +2051,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31">
@@ -2056,7 +2059,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32">
@@ -2064,7 +2067,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33">
@@ -2072,7 +2075,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34">
@@ -2080,7 +2083,874 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>111</v>
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>raw</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>